<commit_message>
update process_files functions and working on css
</commit_message>
<xml_diff>
--- a/uploads/PASREL.xlsx
+++ b/uploads/PASREL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaciri\Desktop\XpathLab\Reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacir\OneDrive\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9EE7CA-CA6A-469A-B2C0-39A88D4D5DC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC713E0-BA31-49A0-BDAF-680CDA71713E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -307,9 +307,6 @@
     <t>Xpath</t>
   </si>
   <si>
-    <t>Donnée du modèle</t>
-  </si>
-  <si>
     <t>/Document/Header/SupplierData/SenderData/CompanyData/OtherId[@OtherIdTypCod='Other'][@OtherIdTypTxt='TAX_ID']/@OtherIdCod , 
 /Document/Header/SupplierData/SenderData/CompanyData/OtherId[@OtherIdTypCod='Other'][@OtherIdTypTxt='LEGAL_ID']/@OtherIdCod</t>
   </si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>buyer.country</t>
+  </si>
+  <si>
+    <t>Donnée du modèle</t>
   </si>
 </sst>
 </file>
@@ -442,12 +442,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,7 +456,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -467,9 +466,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -478,7 +474,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,21 +755,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="51.109375" customWidth="1"/>
     <col min="2" max="2" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -970,279 +964,279 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="42" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="B49" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="B51" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="B52" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="42" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="9" t="s">
+      <c r="B54" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="42" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="42" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -1250,7 +1244,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1258,35 +1252,35 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B64" s="2" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>